<commit_message>
enabled to choose evaluation mode
</commit_message>
<xml_diff>
--- a/tests/ast/big_formula.xlsx
+++ b/tests/ast/big_formula.xlsx
@@ -398,21 +398,21 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1">
         <v>10</v>
       </c>
       <c r="C1">
         <f>A1*B1</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -428,15 +428,15 @@
       </c>
       <c r="D2">
         <f>SUM(Liste)</f>
-        <v>4320</v>
+        <v>4310</v>
       </c>
       <c r="E2">
         <f>SUM(A1:A3)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <f>D2-D6+Sum</f>
-        <v>4072</v>
+        <v>4061</v>
       </c>
     </row>
     <row r="3" spans="1:7">

</xml_diff>